<commit_message>
Se agregan archivos de apoyo
</commit_message>
<xml_diff>
--- a/modulo-5/validacion checklist.xlsx
+++ b/modulo-5/validacion checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cesar Arnaez Flores\Desktop\Kibernum\Data Enginnering\modulo 5\repositorio\data-engineer\modulo-5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FBA45A7-26AF-4FB9-8A41-9B8AC33219FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76BF02C-9955-4230-9E12-F510354B938E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9715D8C5-53D6-48E6-9CB6-DA8B6642E621}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Criterio a evaluar</t>
   </si>
@@ -44,31 +44,16 @@
     <t>¿Todos los campos críticos están completos?</t>
   </si>
   <si>
-    <t>Ej. 20% de direcciones faltan</t>
-  </si>
-  <si>
     <t>¿Hay datos duplicados?</t>
   </si>
   <si>
-    <t>Se repiten 15 RUT de clientes</t>
-  </si>
-  <si>
     <t>¿Los formatos cumplen lo esperado?</t>
   </si>
   <si>
-    <t>Correos inválidos detectados</t>
-  </si>
-  <si>
     <t>¿Se puede rastrear el origen de los datos?</t>
   </si>
   <si>
-    <t>Falta historial de edición</t>
-  </si>
-  <si>
     <t>¿Los datos están actualizados?</t>
-  </si>
-  <si>
-    <t>Teléfonos no vigentes</t>
   </si>
   <si>
     <t>Si Cumple</t>
@@ -160,7 +145,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="5">
     <dxf>
       <font>
         <b val="0"/>
@@ -266,111 +251,6 @@
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Segoe UI Symbol"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{0417FA29-78FA-4A13-93AC-8FF0FAFDF519}">
-          <xfpb:DXFComplement i="0"/>
-        </ext>
-      </extLst>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -407,21 +287,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8337EF22-9BB5-4B73-99C4-980773D6F2F1}" name="Tabla1" displayName="Tabla1" ref="A1:D6" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:D6" xr:uid="{8337EF22-9BB5-4B73-99C4-980773D6F2F1}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B506B09B-15A1-4E59-B43E-EE540E544A0C}" name="Criterio a evaluar" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{56748C16-4E3A-4ED5-9507-12BEA7A7D869}" name="Si Cumple" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{40F258B9-F509-4EE3-9F5B-AB75B0EA2E9B}" name="No Cumple" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{CBBD1BAE-6A6C-4546-BEE8-6D110DE25D28}" name="Comentario o hallazgo (Ejemplo)" dataDxfId="6"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1D60C996-D905-43F9-B96E-27D8E98E7684}" name="Tabla13" displayName="Tabla13" ref="A10:D15" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A10:D15" xr:uid="{1D60C996-D905-43F9-B96E-27D8E98E7684}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1D60C996-D905-43F9-B96E-27D8E98E7684}" name="Tabla13" displayName="Tabla13" ref="A2:D7" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A2:D7" xr:uid="{1D60C996-D905-43F9-B96E-27D8E98E7684}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{BF490C23-3460-4CC0-B9A1-CB9DAA2E14CF}" name="Criterio a evaluar" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{CA58765B-D21C-4756-BE04-9702A8A7E839}" name="Si Cumple" dataDxfId="2"/>
@@ -749,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F69DD0-44E6-4211-B519-D679FE4D79C7}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,169 +629,84 @@
     <col min="4" max="4" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="2" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2"/>
     </row>
-    <row r="4" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="2"/>
+      <c r="B7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>